<commit_message>
tests: updated test cases
</commit_message>
<xml_diff>
--- a/tests/data/car_dms_rules_deprecated.xlsx
+++ b/tests/data/car_dms_rules_deprecated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9B0377-3EB0-DB48-BF15-23129165799D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2E26FE-079F-4E60-90DC-F7FF1B36C0CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="42700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41172" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -620,13 +620,13 @@
   <sheetViews>
     <sheetView zoomScale="285" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -634,7 +634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -642,7 +642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -650,7 +650,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -658,17 +658,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -676,7 +676,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -684,7 +684,7 @@
         <v>45695.809878616063</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -692,12 +692,12 @@
         <v>45695.809878616303</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -711,26 +711,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.5" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
     <col min="3" max="4" width="13" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="11" width="13" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5" hidden="1" customWidth="1"/>
-    <col min="13" max="14" width="13" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" customWidth="1"/>
+    <col min="6" max="11" width="13" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" customWidth="1"/>
+    <col min="13" max="14" width="13" customWidth="1"/>
     <col min="15" max="15" width="94.6640625" customWidth="1"/>
     <col min="16" max="16" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -749,7 +748,7 @@
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
     </row>
-    <row r="2" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -799,7 +798,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -822,7 +821,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -854,7 +853,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -889,7 +888,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -921,7 +920,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -962,19 +961,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
     <col min="2" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
@@ -986,7 +985,7 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -1012,7 +1011,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1026,7 +1025,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1040,7 +1039,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1068,14 +1067,14 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" customWidth="1"/>
     <col min="2" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>55</v>
       </c>
@@ -1085,7 +1084,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>27</v>
       </c>
@@ -1105,17 +1104,17 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1134,14 +1133,14 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="1" max="1" width="30.44140625" customWidth="1"/>
     <col min="2" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>57</v>
       </c>
@@ -1150,7 +1149,7 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>58</v>
       </c>
@@ -1181,14 +1180,14 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
     <col min="2" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>60</v>
       </c>
@@ -1197,7 +1196,7 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>61</v>
       </c>
@@ -1214,7 +1213,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>63</v>
       </c>

</xml_diff>